<commit_message>
Highlighting is pretty good now
</commit_message>
<xml_diff>
--- a/test1out.xlsx
+++ b/test1out.xlsx
@@ -45,22 +45,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FFFFDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E8E8FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00FFDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DDDDFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00DDFFDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFDD"/>
       </patternFill>
     </fill>
   </fills>
@@ -80,10 +80,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -499,7 +499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>This is a leading line, before the table</t>
+          <t>Test by running: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --out=test1out.xlsx</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -522,62 +522,62 @@
       <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>c-</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D5" s="1" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="E5" s="4" t="inlineStr">
         <is>
           <t>Origin</t>
         </is>
       </c>
       <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="1" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr"/>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>c+</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr"/>
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="E6" s="3" t="inlineStr"/>
+      <c r="E6" s="4" t="inlineStr"/>
       <c r="F6" s="5" t="inlineStr">
         <is>
           <t>Shape</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
@@ -589,12 +589,12 @@
           <t>-</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>2022-11-01 00:00:00</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -604,7 +604,7 @@
           <t>apple</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E7" s="4" t="inlineStr">
         <is>
           <t>Maine</t>
         </is>
@@ -622,8 +622,8 @@
           <t>+</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr"/>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr"/>
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -633,7 +633,7 @@
           <t>grapes</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr"/>
+      <c r="E8" s="4" t="inlineStr"/>
       <c r="F8" s="5" t="inlineStr">
         <is>
           <t>pebbles</t>
@@ -651,12 +651,12 @@
           <t>c-</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>2022-11-05 00:00:00</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -666,7 +666,7 @@
           <t>banana</t>
         </is>
       </c>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="E9" s="4" t="inlineStr">
         <is>
           <t>Chile</t>
         </is>
@@ -684,8 +684,8 @@
           <t>c+</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr"/>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr"/>
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -695,7 +695,7 @@
           <t>mango</t>
         </is>
       </c>
-      <c r="E10" s="3" t="inlineStr"/>
+      <c r="E10" s="4" t="inlineStr"/>
       <c r="F10" s="5" t="inlineStr">
         <is>
           <t>oval</t>
@@ -713,12 +713,12 @@
           <t>-</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>2022-11-20 00:00:00</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" s="1" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -728,7 +728,7 @@
           <t>coconut</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="E11" s="4" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
@@ -746,8 +746,8 @@
           <t>=</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr"/>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="B12" s="4" t="inlineStr"/>
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -757,7 +757,7 @@
           <t>dried mango</t>
         </is>
       </c>
-      <c r="E12" s="3" t="inlineStr"/>
+      <c r="E12" s="4" t="inlineStr"/>
       <c r="F12" s="5" t="inlineStr">
         <is>
           <t>flat</t>

</xml_diff>

<commit_message>
Fixed bug: 0 values were treated as empty
</commit_message>
<xml_diff>
--- a/test1out.xlsx
+++ b/test1out.xlsx
@@ -76,13 +76,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -448,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,101 +617,105 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr"/>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>grapes</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr"/>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t>pebbles</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>purple</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>c-</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>2022-11-05 00:00:00</t>
         </is>
       </c>
-      <c r="C8" s="1" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D8" s="1" t="inlineStr">
+      <c r="D9" s="1" t="inlineStr">
         <is>
           <t>banana</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
+      <c r="E9" s="4" t="inlineStr">
         <is>
           <t>Chile</t>
         </is>
       </c>
-      <c r="F8" s="5" t="inlineStr"/>
-      <c r="G8" s="1" t="inlineStr">
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t>oval</t>
+        </is>
+      </c>
+      <c r="G9" s="6" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>2022-11-20 00:00:00</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>coconut</t>
-        </is>
-      </c>
-      <c r="E9" s="4" t="inlineStr">
-        <is>
-          <t>Hawaii</t>
-        </is>
-      </c>
-      <c r="F9" s="5" t="inlineStr"/>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>brown</t>
-        </is>
-      </c>
-    </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>c+</t>
         </is>
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>2022-11-21 00:00:00</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="inlineStr">
-        <is>
-          <t>dried mango</t>
+          <t>2022-11-05 00:00:00</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>mango</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
         <is>
-          <t>Thailand</t>
-        </is>
-      </c>
-      <c r="F10" s="5" t="inlineStr"/>
-      <c r="G10" s="1" t="inlineStr">
-        <is>
-          <t>orange</t>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t>oval</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="inlineStr">
+        <is>
+          <t>yellow</t>
         </is>
       </c>
     </row>
@@ -720,112 +725,99 @@
           <t>-</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr"/>
-      <c r="C11" s="1" t="inlineStr"/>
-      <c r="D11" s="1" t="inlineStr"/>
-      <c r="E11" s="1" t="inlineStr"/>
-      <c r="F11" s="1" t="inlineStr"/>
-      <c r="G11" s="1" t="inlineStr"/>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>2022-11-20 00:00:00</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>coconut</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>Hawaii</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="inlineStr"/>
+      <c r="G11" s="1" t="inlineStr">
+        <is>
+          <t>brown</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>2022-11-21 00:00:00</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>dried mango</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>flat</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>orange</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="B12" s="1" t="inlineStr">
+      <c r="B13" s="1" t="inlineStr"/>
+      <c r="C13" s="1" t="inlineStr"/>
+      <c r="D13" s="1" t="inlineStr"/>
+      <c r="E13" s="1" t="inlineStr"/>
+      <c r="F13" s="1" t="inlineStr"/>
+      <c r="G13" s="1" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
         <is>
           <t>Trailing row here</t>
         </is>
       </c>
-      <c r="C12" s="1" t="inlineStr"/>
-      <c r="D12" s="1" t="inlineStr"/>
-      <c r="E12" s="1" t="inlineStr"/>
-      <c r="F12" s="1" t="inlineStr"/>
-      <c r="G12" s="1" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr"/>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>grapes</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>pebbles</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>purple</t>
-        </is>
-      </c>
-      <c r="F13" s="2" t="inlineStr"/>
-      <c r="G13" s="2" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>mango</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>oval</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>yellow</t>
-        </is>
-      </c>
-      <c r="F14" s="2" t="inlineStr"/>
-      <c r="G14" s="2" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>dried mango</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="inlineStr">
-        <is>
-          <t>orange</t>
-        </is>
-      </c>
-      <c r="F15" s="2" t="inlineStr"/>
-      <c r="G15" s="2" t="inlineStr"/>
+      <c r="C14" s="1" t="inlineStr"/>
+      <c r="D14" s="1" t="inlineStr"/>
+      <c r="E14" s="1" t="inlineStr"/>
+      <c r="F14" s="1" t="inlineStr"/>
+      <c r="G14" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Echo command in first diff row
</commit_message>
<xml_diff>
--- a/test1out.xlsx
+++ b/test1out.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,55 +458,55 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --out=test1out.xlsx</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+      <c r="F1" t="inlineStr"/>
+      <c r="G1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Example TableOld</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr"/>
-      <c r="D1" s="1" t="inlineStr"/>
-      <c r="E1" s="1" t="inlineStr"/>
-      <c r="F1" s="1" t="inlineStr"/>
-      <c r="G1" s="1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr"/>
+      <c r="D2" s="1" t="inlineStr"/>
+      <c r="E2" s="1" t="inlineStr"/>
+      <c r="F2" s="1" t="inlineStr"/>
+      <c r="G2" s="1" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Example TableNew</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr"/>
-      <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr"/>
-      <c r="F2" s="2" t="inlineStr"/>
-      <c r="G2" s="2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Test by running: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --out=test1out.xlsx</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="C3" s="2" t="inlineStr"/>
+      <c r="D3" s="2" t="inlineStr"/>
+      <c r="E3" s="2" t="inlineStr"/>
+      <c r="F3" s="2" t="inlineStr"/>
+      <c r="G3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,7 +514,11 @@
           <t>=</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test by running: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --out=test1out.xlsx</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -522,318 +526,318 @@
       <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>c-</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>Fruit</t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>Origin</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>Color</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
+          <t>c-</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>Fruit</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>Origin</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
           <t>c+</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr"/>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr"/>
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>Fruit</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="E7" s="4" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Shape</t>
         </is>
       </c>
-      <c r="G6" s="3" t="inlineStr">
+      <c r="G7" s="3" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
         <is>
           <t>2022-11-01 00:00:00</t>
         </is>
       </c>
-      <c r="C7" s="1" t="inlineStr">
+      <c r="C8" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D7" s="1" t="inlineStr">
+      <c r="D8" s="1" t="inlineStr">
         <is>
           <t>apple</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="E8" s="4" t="inlineStr">
         <is>
           <t>Maine</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="1" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr"/>
+      <c r="G8" s="1" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr"/>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr"/>
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>grapes</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr"/>
-      <c r="F8" s="5" t="inlineStr">
+      <c r="E9" s="4" t="inlineStr"/>
+      <c r="F9" s="5" t="inlineStr">
         <is>
           <t>pebbles</t>
         </is>
       </c>
-      <c r="G8" s="2" t="inlineStr">
+      <c r="G9" s="2" t="inlineStr">
         <is>
           <t>purple</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>c-</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>2022-11-05 00:00:00</t>
-        </is>
-      </c>
-      <c r="C9" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>banana</t>
-        </is>
-      </c>
-      <c r="E9" s="4" t="inlineStr">
-        <is>
-          <t>Chile</t>
-        </is>
-      </c>
-      <c r="F9" s="5" t="inlineStr">
-        <is>
-          <t>oval</t>
-        </is>
-      </c>
-      <c r="G9" s="6" t="inlineStr">
-        <is>
-          <t>yellow</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
+          <t>c-</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>2022-11-05 00:00:00</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>banana</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t>oval</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="inlineStr">
+        <is>
+          <t>yellow</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>c+</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>2022-11-05 00:00:00</t>
         </is>
       </c>
-      <c r="C10" s="6" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>mango</t>
         </is>
       </c>
-      <c r="E10" s="4" t="inlineStr">
+      <c r="E11" s="4" t="inlineStr">
         <is>
           <t>Chile</t>
         </is>
       </c>
-      <c r="F10" s="5" t="inlineStr">
+      <c r="F11" s="5" t="inlineStr">
         <is>
           <t>oval</t>
         </is>
       </c>
-      <c r="G10" s="6" t="inlineStr">
+      <c r="G11" s="6" t="inlineStr">
         <is>
           <t>yellow</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B12" s="4" t="inlineStr">
         <is>
           <t>2022-11-20 00:00:00</t>
         </is>
       </c>
-      <c r="C11" s="1" t="inlineStr">
+      <c r="C12" s="1" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="D11" s="1" t="inlineStr">
+      <c r="D12" s="1" t="inlineStr">
         <is>
           <t>coconut</t>
         </is>
       </c>
-      <c r="E11" s="4" t="inlineStr">
+      <c r="E12" s="4" t="inlineStr">
         <is>
           <t>Hawaii</t>
         </is>
       </c>
-      <c r="F11" s="5" t="inlineStr"/>
-      <c r="G11" s="1" t="inlineStr">
+      <c r="F12" s="5" t="inlineStr"/>
+      <c r="G12" s="1" t="inlineStr">
         <is>
           <t>brown</t>
         </is>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>c-</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>2022-11-21 00:00:00</t>
-        </is>
-      </c>
-      <c r="C12" s="6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D12" s="6" t="inlineStr">
-        <is>
-          <t>dried mango</t>
-        </is>
-      </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Thailand</t>
-        </is>
-      </c>
-      <c r="F12" s="5" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="G12" s="6" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
+          <t>c-</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>2022-11-21 00:00:00</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>dried mango</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr">
+        <is>
+          <t>flat</t>
+        </is>
+      </c>
+      <c r="G13" s="6" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
           <t>c+</t>
         </is>
       </c>
-      <c r="B13" s="4" t="inlineStr">
+      <c r="B14" s="4" t="inlineStr">
         <is>
           <t>2022-11-21 00:00:00</t>
         </is>
       </c>
-      <c r="C13" s="6" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="D13" s="6" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
         <is>
           <t>dried mango</t>
         </is>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E14" s="4" t="inlineStr">
         <is>
           <t>Thailand</t>
         </is>
       </c>
-      <c r="F13" s="5" t="inlineStr">
+      <c r="F14" s="5" t="inlineStr">
         <is>
           <t>flat</t>
         </is>
       </c>
-      <c r="G13" s="2" t="inlineStr">
+      <c r="G14" s="2" t="inlineStr">
         <is>
           <t>orange</t>
         </is>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="B14" s="1" t="inlineStr"/>
-      <c r="C14" s="1" t="inlineStr"/>
-      <c r="D14" s="1" t="inlineStr"/>
-      <c r="E14" s="1" t="inlineStr"/>
-      <c r="F14" s="1" t="inlineStr"/>
-      <c r="G14" s="1" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -841,17 +845,30 @@
           <t>-</t>
         </is>
       </c>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>Trailing row here</t>
-        </is>
-      </c>
+      <c r="B15" s="1" t="inlineStr"/>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr"/>
       <c r="F15" s="1" t="inlineStr"/>
       <c r="G15" s="1" t="inlineStr"/>
     </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Trailing row here</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr"/>
+      <c r="D16" s="1" t="inlineStr"/>
+      <c r="E16" s="1" t="inlineStr"/>
+      <c r="F16" s="1" t="inlineStr"/>
+      <c r="G16" s="1" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>